<commit_message>
with all fields and same sheet
</commit_message>
<xml_diff>
--- a/output/INV-9576E2.xlsx
+++ b/output/INV-9576E2.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishnasai.g.TECHNOVERT\Documents\UiPath\DocumentProcessing_IntelligentOCR300\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishnasai.g.TECHNOVERT\Documents\UiPath\Invoice Processing\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534CC318-7213-482A-B310-D1F502ECD82A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF6DACF-28CD-4942-B53D-66C0A2F548EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{B7D9A4DF-1820-4E0A-9B2C-3D9B314E51D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B7D9A4DF-1820-4E0A-9B2C-3D9B314E51D9}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceTable - Formatted" sheetId="5" r:id="rId1"/>
     <sheet name="InvoiceTable" sheetId="4" r:id="rId2"/>
     <sheet name="Simple Fields - Formatted" sheetId="3" r:id="rId3"/>
     <sheet name="Simple Fields" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>InvoiceNumber</t>
   </si>
@@ -82,7 +81,54 @@
     <t>Monthly Expanses</t>
   </si>
   <si>
-    <t>DAys</t>
+    <t>Vendor Address</t>
+  </si>
+  <si>
+    <t>Billing Name</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Purchase Order Number</t>
+  </si>
+  <si>
+    <t>Net Amount</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Technovert hyderabad Hyderabad,Telangana,500048 India</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Key,Value_x000D_
+"Address Line 1","Technovert hyderabad"_x000D_
+"City","Hyderabad"_x000D_
+"Country","India"_x000D_
+"State / County / Province","Telangana"_x000D_
+"Zip Postal Code","500048"</t>
+  </si>
+  <si>
+    <t>Line Number</t>
+  </si>
+  <si>
+    <t>Item PO Number</t>
   </si>
 </sst>
 </file>
@@ -118,9 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,13 +484,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F0D9FE-86BE-495D-982A-80D0C720BBE9}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -454,14 +513,17 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>800</v>
-      </c>
       <c r="C2">
         <v>5</v>
       </c>
@@ -469,13 +531,10 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
       <c r="C3">
         <v>5</v>
       </c>
@@ -483,13 +542,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
         <v>780</v>
       </c>
@@ -497,10 +553,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>89</v>
       </c>
@@ -518,13 +571,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913228AB-8523-4D75-8CD6-C2F4FDE1A6A3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -537,14 +599,17 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>800</v>
-      </c>
       <c r="C2">
         <v>5</v>
       </c>
@@ -552,13 +617,10 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
       <c r="C3">
         <v>5</v>
       </c>
@@ -566,13 +628,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
         <v>780</v>
       </c>
@@ -580,10 +639,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>89</v>
       </c>
@@ -601,13 +657,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFAD482-8952-4436-8972-5B8883F06FDF}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,8 +686,38 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -639,6 +732,21 @@
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1">
+        <v>43727</v>
+      </c>
+      <c r="M2">
+        <v>4828.01</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -648,13 +756,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34513A30-BBEF-4806-A692-D9FDBCE9D36D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,8 +784,38 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -686,21 +830,24 @@
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1">
+        <v>43727</v>
+      </c>
+      <c r="M2">
+        <v>4828.01</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E368C7-AF0F-45AD-99F4-F3506FA77A5A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>